<commit_message>
Updating simulation test values
</commit_message>
<xml_diff>
--- a/Scenario 1_test.xlsx
+++ b/Scenario 1_test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdlatour\AppData\Local\Temp\scp29210\local\users\cdlatour\Multiple_outcomes_pregnancy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEF80F0-3C1F-8147-AC51-61FC975953BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="820" windowWidth="28800" windowHeight="16220" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="28800" yWindow="825" windowWidth="28800" windowHeight="16215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="OLD" sheetId="1" r:id="rId6"/>
     <sheet name="SB_Risk_Preeclampsia" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,17 +41,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={2D0EDF39-7EAE-8B42-8A25-E31D9B0584A4}</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{2D0EDF39-7EAE-8B42-8A25-E31D9B0584A4}">
+    <comment ref="E6" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Everyone who has a continuing pregnancy is indexed at week 4. By having more rows, we allow for subsequent simulations where people can be indexed at different gestational weeks.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -60,26 +68,44 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={6F0D0981-BCCC-D340-9528-F44FC96324E0}</author>
     <author>tc={5F2D1E39-8D5C-0A4A-B365-BF113D93EECC}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{6F0D0981-BCCC-D340-9528-F44FC96324E0}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     DECREASES the risk of fetal death, starting at gestational week 4 from conception (i.e., the week that everyone is indexed into the trial if they have continued their pregnancy.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="1" shapeId="0" xr:uid="{5F2D1E39-8D5C-0A4A-B365-BF113D93EECC}">
+    <comment ref="D26" authorId="1" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     DECREASES the risk of preterm birth, RR = 0.7, and subsequently increases the risk of term births (&gt;= 35 weeks from conception), RR = 1.05</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -87,7 +113,7 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={64BAD85A-477D-3B47-ACFB-F7563888EB93}</author>
     <author>tc={4842E7A7-EBD7-CE4B-AB5E-5EFBBB07D91E}</author>
@@ -95,38 +121,74 @@
     <author>tc={DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{64BAD85A-477D-3B47-ACFB-F7563888EB93}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This information is based upon the following. https://www.sciencedirect.com/science/article/pii/S0002937813008594?via%3Dihub#fig1</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{4842E7A7-EBD7-CE4B-AB5E-5EFBBB07D91E}">
+    <comment ref="C1" authorId="1" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Increased the risk of preeclampsia for the simulation — Individuals with CH are at much higher risk of preeclampsia (e.g., 10-25%) than those without: High blood pressure: A risk factor for preeclampsiaMarch of Dimeshttps://www.marchofdimes.org › find-support › blog › h...</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{8166E600-F91C-DF49-B3FC-30F8863F4314}">
+    <comment ref="E1" authorId="2" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Treatment DECREASES the odds of preeclampsia</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="3" shapeId="0" xr:uid="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
+    <comment ref="G1" authorId="3" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/
 Reply:
     Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -134,17 +196,26 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={D251C841-2558-B642-82DC-6ED550C61FF7}</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{D251C841-2558-B642-82DC-6ED550C61FF7}">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Treatment DECREASES risk of SGA, RR = 0.8</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -152,17 +223,26 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={EB10B5D4-D174-9E46-AE4A-935ECC1C8009}</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{EB10B5D4-D174-9E46-AE4A-935ECC1C8009}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Very minimal uninformative censoring.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -170,7 +250,7 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={E6E88FEF-63DE-2F45-80DF-11FAF199CED4}</author>
     <author>tc={B831F326-F008-1346-B1B1-8CC11324C357}</author>
@@ -181,61 +261,124 @@
     <author>tc={922FBB19-8B5B-A34B-A9B0-54F331113989}</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E6E88FEF-63DE-2F45-80DF-11FAF199CED4}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{B831F326-F008-1346-B1B1-8CC11324C357}">
+    <comment ref="E1" authorId="1" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Going to assume that once someone develops severe preeclampsia that they </t>
+        </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="2" shapeId="0" xr:uid="{DDBB59B4-2F6E-C04D-8EA2-09D2C1914C68}">
+    <comment ref="B17" authorId="2" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="3" shapeId="0" xr:uid="{E9BCC1D5-1B59-E946-915C-60D136876422}">
+    <comment ref="C22" authorId="3" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="4" shapeId="0" xr:uid="{7FD7AEEF-71D2-574A-9052-EA48BC9A0990}">
+    <comment ref="E22" authorId="4" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.sciencedirect.com/science/article/pii/S0002937813008594?via%3Dihub#fig1</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="5" shapeId="0" xr:uid="{24ECC65E-7926-A74D-88BA-ECF06281649B}">
+    <comment ref="F22" authorId="5" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.cdc.gov/nchs/data/vsrr/vsrr021.pdf
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="6" shapeId="0" xr:uid="{922FBB19-8B5B-A34B-A9B0-54F331113989}">
+    <comment ref="B33" authorId="6" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -243,36 +386,63 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={7F21C0C9-3748-7449-8B61-7AC75D94AA52}</author>
     <author>tc={760167DC-12EB-F840-B9E8-A3B42A8E8484}</author>
     <author>tc={895E85A6-7599-BE4D-A5A6-2C2F9CEB3D46}</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7F21C0C9-3748-7449-8B61-7AC75D94AA52}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/#:~:text=However%2C%20relative%20risk%20of%20stillbirth,CI%3D46%20to%20142).</t>
+        </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="1" shapeId="0" xr:uid="{760167DC-12EB-F840-B9E8-A3B42A8E8484}">
+    <comment ref="L2" authorId="1" shapeId="0">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The values that going to use, given statistical probs. Assuming that preeclampsia leads to at least as high a probability of fetal death. Going to take the maximimum of the risk here and the risk that we’re using in Phase 1
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="K18" authorId="2" shapeId="0" xr:uid="{895E85A6-7599-BE4D-A5A6-2C2F9CEB3D46}">
+    <comment ref="K18" authorId="2" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -396,7 +566,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -453,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -462,6 +632,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -892,23 +1065,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -928,20 +1101,20 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <f>0.9*F2</f>
-        <v>9.0000000000000011E-2</v>
+        <f>0.5*F2</f>
+        <v>0.05</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
         <f>1-C2-B2</f>
-        <v>0.91</v>
+        <v>0.95</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -950,20 +1123,20 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B42" si="0">0.9*F3</f>
-        <v>9.0000000000000011E-2</v>
+      <c r="B3" s="8">
+        <f t="shared" ref="B3:B42" si="0">0.5*F3</f>
+        <v>0.05</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <f>1-C3-B3</f>
-        <v>0.91</v>
+        <v>0.95</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -972,20 +1145,20 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>4.5000000000000005E-2</v>
+      <c r="B4" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
         <f>1-C4-B4</f>
-        <v>0.95499999999999996</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -994,20 +1167,20 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>4.5000000000000005E-2</v>
+      <c r="B5" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
         <f>1-C5-B5</f>
-        <v>0.95499999999999996</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1016,20 +1189,20 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>4.5000000000000005E-2</v>
+      <c r="B6" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
         <f>1-C6-B6</f>
-        <v>0.95499999999999996</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1038,20 +1211,20 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>4.5000000000000005E-2</v>
+      <c r="B7" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D41" si="1">1-B7-C7</f>
-        <v>0.95499999999999996</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1060,20 +1233,20 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>2.7E-2</v>
+      <c r="B8" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>0.97299999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1082,20 +1255,20 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>2.7E-2</v>
+      <c r="B9" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>0.97299999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1104,20 +1277,20 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>2.7E-2</v>
+      <c r="B10" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>0.97299999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1126,20 +1299,20 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>2.7E-2</v>
+      <c r="B11" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>0.97299999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1148,20 +1321,20 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>2.7E-2</v>
+      <c r="B12" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>0.97299999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1170,20 +1343,20 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>2.7E-2</v>
+      <c r="B13" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>0.97299999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1192,20 +1365,20 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>9.0000000000000011E-3</v>
+      <c r="B14" s="8">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>0.99099999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1214,20 +1387,20 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>9.0000000000000011E-3</v>
+      <c r="B15" s="8">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>0.99099999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1236,20 +1409,20 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>9.0000000000000011E-3</v>
+      <c r="B16" s="8">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>0.99099999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1258,20 +1431,20 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>9.0000000000000011E-3</v>
+      <c r="B17" s="8">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>0.99099999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1280,20 +1453,20 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>9.0000000000000011E-3</v>
+      <c r="B18" s="8">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>0.99099999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1302,20 +1475,20 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>9.0000000000000011E-3</v>
+      <c r="B19" s="8">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>0.99099999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1324,20 +1497,20 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>9.0000000000000011E-3</v>
+      <c r="B20" s="8">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>0.99099999999999999</v>
+        <v>0.995</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1346,20 +1519,20 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B21" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>0.99729999999999996</v>
+        <v>0.99850000000000005</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1368,20 +1541,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B22" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>0.99729999999999996</v>
+        <v>0.99850000000000005</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1390,20 +1563,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B23" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>0.99729999999999996</v>
+        <v>0.99850000000000005</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1412,20 +1585,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B24" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>0.99729999999999996</v>
+        <v>0.99850000000000005</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1434,20 +1607,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B25" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>0.99729999999999996</v>
+        <v>0.99850000000000005</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1456,20 +1629,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B26" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C26">
         <v>0.01</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>0.98729999999999996</v>
+        <v>0.98850000000000005</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1478,20 +1651,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B27" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C27">
         <v>0.01</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>0.98729999999999996</v>
+        <v>0.98850000000000005</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1500,20 +1673,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B28" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C28">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
-        <v>0.98229999999999995</v>
+        <v>0.98350000000000004</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1522,20 +1695,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B29" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C29">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
-        <v>0.98229999999999995</v>
+        <v>0.98350000000000004</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1544,20 +1717,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B30" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C30">
         <v>0.02</v>
       </c>
       <c r="D30">
         <f t="shared" si="1"/>
-        <v>0.97729999999999995</v>
+        <v>0.97850000000000004</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1566,20 +1739,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B31" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C31">
         <v>0.02</v>
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
-        <v>0.97729999999999995</v>
+        <v>0.97850000000000004</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1588,20 +1761,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B32" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C32">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D32">
         <f t="shared" si="1"/>
-        <v>0.97229999999999994</v>
+        <v>0.97350000000000003</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1610,20 +1783,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B33" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C33">
         <v>0.03</v>
       </c>
       <c r="D33">
         <f t="shared" si="1"/>
-        <v>0.96729999999999994</v>
+        <v>0.96850000000000003</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1632,20 +1805,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B34" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C34">
         <v>0.09</v>
       </c>
       <c r="D34">
         <f t="shared" si="1"/>
-        <v>0.9073</v>
+        <v>0.90850000000000009</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1654,20 +1827,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B35" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C35">
         <v>0.09</v>
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
-        <v>0.9073</v>
+        <v>0.90850000000000009</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1676,20 +1849,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000001E-3</v>
+      <c r="B36" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
       </c>
       <c r="C36">
         <v>0.09</v>
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
-        <v>0.9073</v>
+        <v>0.90850000000000009</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1698,20 +1871,20 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37">
-        <f t="shared" si="0"/>
-        <v>1.8900000000000001E-4</v>
+      <c r="B37" s="8">
+        <f t="shared" si="0"/>
+        <v>1.05E-4</v>
       </c>
       <c r="C37">
         <v>0.3</v>
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
-        <v>0.69981099999999996</v>
+        <v>0.69989499999999993</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1721,20 +1894,20 @@
         <v>2.1000000000000001E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38">
-        <f t="shared" si="0"/>
-        <v>2.43E-4</v>
+      <c r="B38" s="8">
+        <f t="shared" si="0"/>
+        <v>1.35E-4</v>
       </c>
       <c r="C38">
         <v>0.35</v>
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
-        <v>0.64975700000000003</v>
+        <v>0.64986500000000003</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1743,20 +1916,20 @@
         <v>2.7E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39">
-        <f t="shared" si="0"/>
-        <v>3.1500000000000001E-4</v>
+      <c r="B39" s="8">
+        <f t="shared" si="0"/>
+        <v>1.75E-4</v>
       </c>
       <c r="C39">
         <v>0.7</v>
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
-        <v>0.29968500000000009</v>
+        <v>0.29982500000000001</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1765,20 +1938,20 @@
         <v>3.5E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40">
-        <f t="shared" si="0"/>
-        <v>3.7800000000000003E-4</v>
+      <c r="B40" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1000000000000001E-4</v>
       </c>
       <c r="C40">
         <v>0.7</v>
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
-        <v>0.29962200000000005</v>
+        <v>0.29979</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1787,20 +1960,20 @@
         <v>4.2000000000000002E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41">
-        <f t="shared" si="0"/>
-        <v>5.4900000000000001E-4</v>
+      <c r="B41" s="8">
+        <f t="shared" si="0"/>
+        <v>3.0499999999999999E-4</v>
       </c>
       <c r="C41">
         <v>0.7</v>
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
-        <v>0.29945100000000002</v>
+        <v>0.29969500000000004</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1809,17 +1982,17 @@
         <v>6.0999999999999997E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42">
-        <f t="shared" si="0"/>
-        <v>9.7199999999999999E-4</v>
+      <c r="B42" s="8">
+        <f t="shared" si="0"/>
+        <v>5.4000000000000001E-4</v>
       </c>
       <c r="C42">
         <f>1-B42</f>
-        <v>0.99902800000000003</v>
+        <v>0.99946000000000002</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1838,23 +2011,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.375" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1871,7 +2044,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1889,7 +2062,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1907,7 +2080,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1925,7 +2098,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1943,7 +2116,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1952,607 +2125,607 @@
       </c>
       <c r="C6">
         <f>0.8*Phase1!B6</f>
-        <v>3.6000000000000004E-2</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6" si="1">1-D6-C6</f>
-        <v>0.96399999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <f>0.8*Phase1!B7</f>
-        <v>3.6000000000000004E-2</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E41" si="2">1-C7-D7</f>
-        <v>0.96399999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <f>0.8*Phase1!B8</f>
-        <v>2.1600000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>0.97840000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <f>0.8*Phase1!B9</f>
-        <v>2.1600000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>0.97840000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <f>0.8*Phase1!B10</f>
-        <v>2.1600000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>0.97840000000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <f>0.8*Phase1!B11</f>
-        <v>2.1600000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>0.97840000000000005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <f>0.8*Phase1!B12</f>
-        <v>2.1600000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>0.97840000000000005</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <f>0.8*Phase1!B13</f>
-        <v>2.1600000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>0.97840000000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98799999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <f>0.8*Phase1!B14</f>
-        <v>7.2000000000000015E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>0.99280000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <f>0.8*Phase1!B15</f>
-        <v>7.2000000000000015E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>0.99280000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <f>0.8*Phase1!B16</f>
-        <v>7.2000000000000015E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>0.99280000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <f>0.8*Phase1!B17</f>
-        <v>7.2000000000000015E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>0.99280000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <f>0.8*Phase1!B18</f>
-        <v>7.2000000000000015E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
-        <v>0.99280000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <f>0.8*Phase1!B19</f>
-        <v>7.2000000000000015E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>0.99280000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <f>0.8*Phase1!B20</f>
-        <v>7.2000000000000015E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>0.99280000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <f>0.8*Phase1!B21</f>
-        <v>2.16E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>0.99783999999999995</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.99880000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <f>0.8*Phase1!B22</f>
-        <v>2.16E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
-        <v>0.99783999999999995</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.99880000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <f>0.8*Phase1!B23</f>
-        <v>2.16E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>0.99783999999999995</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.99880000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <f>0.8*Phase1!B24</f>
-        <v>2.16E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>0.99783999999999995</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.99880000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <f>0.8*Phase1!B25</f>
-        <v>2.16E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>0.99783999999999995</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.99880000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <f>0.8*Phase1!B26</f>
-        <v>2.16E-3</v>
+        <v>1.2000000000000001E-3</v>
       </c>
       <c r="D26">
-        <f>0.7*Phase1!C26</f>
-        <v>6.9999999999999993E-3</v>
+        <f>0.8*Phase1!C26</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
-        <v>0.99083999999999994</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.99080000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <f>0.8*Phase1!B27</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D27">
-        <f>0.7*Phase1!C27</f>
-        <v>6.9999999999999993E-3</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D27" s="7">
+        <f>0.8*Phase1!C27</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="E27">
         <f t="shared" si="2"/>
-        <v>0.99083999999999994</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.99080000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <f>0.8*Phase1!B28</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D28">
-        <f>0.7*Phase1!C28</f>
-        <v>1.0499999999999999E-2</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D28" s="7">
+        <f>0.8*Phase1!C28</f>
+        <v>1.2E-2</v>
       </c>
       <c r="E28">
         <f t="shared" si="2"/>
-        <v>0.98734</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98680000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <f>0.8*Phase1!B29</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D29">
-        <f>0.7*Phase1!C29</f>
-        <v>1.0499999999999999E-2</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D29" s="7">
+        <f>0.8*Phase1!C29</f>
+        <v>1.2E-2</v>
       </c>
       <c r="E29">
         <f t="shared" si="2"/>
-        <v>0.98734</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98680000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <f>0.8*Phase1!B30</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D30">
-        <f>0.7*Phase1!C30</f>
-        <v>1.3999999999999999E-2</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D30" s="7">
+        <f>0.8*Phase1!C30</f>
+        <v>1.6E-2</v>
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
-        <v>0.98383999999999994</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98280000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <f>0.8*Phase1!B31</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D31">
-        <f>0.7*Phase1!C31</f>
-        <v>1.3999999999999999E-2</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D31" s="7">
+        <f>0.8*Phase1!C31</f>
+        <v>1.6E-2</v>
       </c>
       <c r="E31">
         <f t="shared" si="2"/>
-        <v>0.98383999999999994</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98280000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <f>0.8*Phase1!B32</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D32">
-        <f>0.7*Phase1!C32</f>
-        <v>1.7499999999999998E-2</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D32" s="7">
+        <f>0.8*Phase1!C32</f>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="E32">
         <f t="shared" si="2"/>
-        <v>0.98033999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.9788</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="6">
         <f>0.8*Phase1!B33</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D33">
-        <f>0.7*Phase1!C33</f>
-        <v>2.0999999999999998E-2</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D33" s="7">
+        <f>0.8*Phase1!C33</f>
+        <v>2.4E-2</v>
       </c>
       <c r="E33">
         <f t="shared" si="2"/>
-        <v>0.97683999999999993</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.9748</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="6">
         <f>0.8*Phase1!B34</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D34">
-        <f>0.7*Phase1!C34</f>
-        <v>6.3E-2</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D34" s="7">
+        <f>0.8*Phase1!C34</f>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="E34">
         <f t="shared" si="2"/>
-        <v>0.93483999999999989</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.92680000000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="6">
         <f>0.8*Phase1!B35</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D35">
-        <f>0.7*Phase1!C35</f>
-        <v>6.3E-2</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D35" s="7">
+        <f>0.8*Phase1!C35</f>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="E35">
         <f t="shared" si="2"/>
-        <v>0.93483999999999989</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.92680000000000007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="6">
         <f>0.8*Phase1!B36</f>
-        <v>2.16E-3</v>
-      </c>
-      <c r="D36">
-        <f>0.7*Phase1!C36</f>
-        <v>6.3E-2</v>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="D36" s="7">
+        <f>0.8*Phase1!C36</f>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="E36">
         <f t="shared" si="2"/>
-        <v>0.93483999999999989</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.92680000000000007</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="6">
         <f>0.8*Phase1!B37</f>
-        <v>1.5120000000000002E-4</v>
+        <v>8.4000000000000009E-5</v>
       </c>
       <c r="D37">
         <f>1.05*Phase1!C37</f>
@@ -2560,19 +2733,19 @@
       </c>
       <c r="E37">
         <f t="shared" si="2"/>
-        <v>0.68484879999999992</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.68491600000000008</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="6">
         <f>0.8*Phase1!B38</f>
-        <v>1.9440000000000001E-4</v>
+        <v>1.0800000000000001E-4</v>
       </c>
       <c r="D38">
         <f>1.05*Phase1!C38</f>
@@ -2580,19 +2753,19 @@
       </c>
       <c r="E38">
         <f t="shared" si="2"/>
-        <v>0.63230560000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.63239200000000007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="6">
         <f>0.8*Phase1!B39</f>
-        <v>2.52E-4</v>
+        <v>1.4000000000000001E-4</v>
       </c>
       <c r="D39">
         <f>1.05*Phase1!C39</f>
@@ -2600,19 +2773,19 @@
       </c>
       <c r="E39">
         <f t="shared" si="2"/>
-        <v>0.26474799999999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.26485999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="6">
         <f>0.8*Phase1!B40</f>
-        <v>3.0240000000000003E-4</v>
+        <v>1.6800000000000002E-4</v>
       </c>
       <c r="D40">
         <f>1.05*Phase1!C40</f>
@@ -2620,19 +2793,19 @@
       </c>
       <c r="E40">
         <f t="shared" si="2"/>
-        <v>0.26469759999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.26483200000000007</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="6">
         <f>0.8*Phase1!B41</f>
-        <v>4.3920000000000005E-4</v>
+        <v>2.4399999999999999E-4</v>
       </c>
       <c r="D41">
         <f>1.05*Phase1!C41</f>
@@ -2640,23 +2813,23 @@
       </c>
       <c r="E41">
         <f t="shared" si="2"/>
-        <v>0.26456080000000004</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.26475599999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="6">
         <f>0.8*Phase1!B42</f>
-        <v>7.7760000000000004E-4</v>
+        <v>4.3200000000000004E-4</v>
       </c>
       <c r="D42">
         <f>1-C42</f>
-        <v>0.99922239999999996</v>
+        <v>0.99956800000000001</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2669,26 +2842,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCEC42C-213B-4245-8F9C-C0F65FBC0D09}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="20.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.125" customWidth="1"/>
+    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2714,7 +2887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>24</v>
       </c>
@@ -2722,19 +2895,19 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C2">
-        <f>10*B2</f>
-        <v>4.0000000000000001E-3</v>
+        <f>16*B2</f>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="D2">
         <f>LN(C2/(1-C2))</f>
-        <v>-5.5174528964647074</v>
+        <v>-5.045036720813588</v>
       </c>
       <c r="E2">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="F2">
         <f>LN(E2)</f>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G2">
         <v>1.7000000000000001E-2</v>
@@ -2744,27 +2917,27 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25</v>
       </c>
       <c r="B3">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C18" si="1">10*B3</f>
-        <v>4.0000000000000001E-3</v>
+      <c r="C3" s="8">
+        <f t="shared" ref="C3:C18" si="1">16*B3</f>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="D3">
         <f>LN(C3/(1-C3))</f>
-        <v>-5.5174528964647074</v>
-      </c>
-      <c r="E3">
-        <v>0.4</v>
+        <v>-5.045036720813588</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.6</v>
       </c>
       <c r="F3">
         <f>LN(E3)</f>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G3">
         <v>1.7000000000000001E-2</v>
@@ -2774,27 +2947,27 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>26</v>
       </c>
       <c r="B4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C4">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
+      <c r="C4" s="8">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D18" si="2">LN(C4/(1-C4))</f>
-        <v>-5.2933048247244923</v>
-      </c>
-      <c r="E4">
-        <v>0.4</v>
+        <v>-4.8202815656050371</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.6</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F18" si="3">LN(E4)</f>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G4">
         <v>3.0000000000000001E-3</v>
@@ -2804,27 +2977,27 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>27</v>
       </c>
       <c r="B5">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
-        <v>5.9999999999999993E-3</v>
+      <c r="C5" s="8">
+        <f t="shared" si="1"/>
+        <v>9.5999999999999992E-3</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>-5.1099777374285189</v>
-      </c>
-      <c r="E5">
-        <v>0.4</v>
+        <v>-4.6363458034565408</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.6</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G5">
         <v>4.0000000000000001E-3</v>
@@ -2834,27 +3007,27 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>28</v>
       </c>
       <c r="B6">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000001E-3</v>
+      <c r="C6" s="8">
+        <f t="shared" si="1"/>
+        <v>1.12E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>-4.9548205149898594</v>
-      </c>
-      <c r="E6">
-        <v>0.4</v>
+        <v>-4.4805783084023778</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.6</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G6">
         <v>3.0000000000000001E-3</v>
@@ -2864,27 +3037,27 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>29</v>
       </c>
       <c r="B7">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+      <c r="C7" s="8">
+        <f t="shared" si="1"/>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>-4.8202815656050371</v>
-      </c>
-      <c r="E7">
-        <v>0.4</v>
+        <v>-4.3454274822255519</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.6</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G7">
         <v>3.0000000000000001E-3</v>
@@ -2894,27 +3067,27 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
       <c r="B8">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
-        <v>8.9999999999999993E-3</v>
+      <c r="C8" s="8">
+        <f t="shared" si="1"/>
+        <v>1.44E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>-4.7014899569937691</v>
-      </c>
-      <c r="E8">
-        <v>0.4</v>
+        <v>-4.2260223861973003</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.6</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G8">
         <v>3.0000000000000001E-3</v>
@@ -2924,27 +3097,27 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>31</v>
       </c>
       <c r="B9">
         <v>1E-3</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+      <c r="C9" s="8">
+        <f t="shared" si="1"/>
+        <v>1.6E-2</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>-4.5951198501345898</v>
-      </c>
-      <c r="E9">
-        <v>0.4</v>
+        <v>-4.1190371748124717</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.6</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G9">
         <v>3.0000000000000001E-3</v>
@@ -2954,27 +3127,27 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>32</v>
       </c>
       <c r="B10">
         <v>1.8E-3</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
-        <v>1.7999999999999999E-2</v>
+      <c r="C10" s="8">
+        <f t="shared" si="1"/>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>-3.9992195504583012</v>
-      </c>
-      <c r="E10">
-        <v>0.4</v>
+        <v>-3.5181570331633334</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.6</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G10">
         <v>3.0000000000000001E-3</v>
@@ -2984,27 +3157,27 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>33</v>
       </c>
       <c r="B11">
         <v>2E-3</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
+      <c r="C11" s="8">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>-3.8918202981106265</v>
-      </c>
-      <c r="E11">
-        <v>0.4</v>
+        <v>-3.4094961844768505</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.6</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G11">
         <v>3.0000000000000001E-3</v>
@@ -3014,27 +3187,27 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>34</v>
       </c>
       <c r="B12">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
-        <v>0.04</v>
+      <c r="C12" s="8">
+        <f t="shared" si="1"/>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>-3.1780538303479453</v>
-      </c>
-      <c r="E12">
-        <v>0.4</v>
+        <v>-2.6827323931179201</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.6</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G12">
         <v>3.0000000000000001E-3</v>
@@ -3044,27 +3217,27 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>35</v>
       </c>
       <c r="B13">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
-        <v>0.05</v>
+      <c r="C13" s="8">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>-2.9444389791664403</v>
-      </c>
-      <c r="E13">
-        <v>0.4</v>
+        <v>-2.4423470353692043</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.6</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G13">
         <v>1E-3</v>
@@ -3074,27 +3247,27 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>36</v>
       </c>
       <c r="B14">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
+      <c r="C14" s="8">
+        <f t="shared" si="1"/>
+        <v>0.112</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>-2.5866893440979424</v>
-      </c>
-      <c r="E14">
-        <v>0.4</v>
+        <v>-2.0704728716970755</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.6</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G14">
         <v>1E-3</v>
@@ -3104,27 +3277,27 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>37</v>
       </c>
       <c r="B15">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
+      <c r="C15" s="8">
+        <f t="shared" si="1"/>
+        <v>0.128</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>-2.4423470353692043</v>
-      </c>
-      <c r="E15">
-        <v>0.4</v>
+        <v>-1.9187591599893623</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.6</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G15">
         <v>1E-3</v>
@@ -3134,27 +3307,27 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>38</v>
       </c>
       <c r="B16">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>8.9999999999999993E-3</v>
+      <c r="C16" s="8">
+        <f t="shared" si="1"/>
+        <v>1.44E-2</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>-4.7014899569937691</v>
-      </c>
-      <c r="E16">
-        <v>0.4</v>
+        <v>-4.2260223861973003</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.6</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G16">
         <v>1E-3</v>
@@ -3164,27 +3337,27 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>39</v>
       </c>
       <c r="B17">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
-        <v>0.10999999999999999</v>
+      <c r="C17" s="8">
+        <f t="shared" si="1"/>
+        <v>0.17599999999999999</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>-2.0907410969337694</v>
-      </c>
-      <c r="E17">
-        <v>0.4</v>
+        <v>-1.54368653487132</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.6</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G17">
         <v>2E-3</v>
@@ -3194,27 +3367,27 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>40</v>
       </c>
       <c r="B18">
         <v>1.4E-2</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
+      <c r="C18" s="8">
+        <f t="shared" si="1"/>
+        <v>0.224</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>-1.8152899666382492</v>
-      </c>
-      <c r="E18">
-        <v>0.4</v>
+        <v>-1.242506468328179</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.6</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
-        <v>-0.916290731874155</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G18">
         <v>1E-3</v>
@@ -3231,20 +3404,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B136535-DC0E-F74A-BC9C-9C0291FB9B47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
@@ -3255,7 +3428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3266,7 +3439,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3278,7 +3451,7 @@
         <v>0.15625</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3290,7 +3463,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3309,20 +3482,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638C0E0C-D6E1-F442-8735-4FA62BD9AC1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -3330,7 +3503,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3338,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3346,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3354,7 +3527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3362,7 +3535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3370,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3378,284 +3551,284 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B40" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42">
-        <v>0</v>
+      <c r="B42" s="7">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3665,21 +3838,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFC6947-DBBF-D243-8019-94691EC417BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22:E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3699,7 +3872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -3720,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
@@ -3741,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -3762,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -3783,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -3804,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
@@ -3825,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -3846,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13</v>
       </c>
@@ -3867,7 +4040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14</v>
       </c>
@@ -3888,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -3909,7 +4082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
@@ -3930,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>17</v>
       </c>
@@ -3951,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>18</v>
       </c>
@@ -3972,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>19</v>
       </c>
@@ -3993,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20</v>
       </c>
@@ -4014,7 +4187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>21</v>
       </c>
@@ -4035,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>22</v>
       </c>
@@ -4056,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>23</v>
       </c>
@@ -4077,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>24</v>
       </c>
@@ -4098,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>25</v>
       </c>
@@ -4119,7 +4292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>26</v>
       </c>
@@ -4140,7 +4313,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>27</v>
       </c>
@@ -4161,7 +4334,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>28</v>
       </c>
@@ -4182,7 +4355,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>29</v>
       </c>
@@ -4203,7 +4376,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>30</v>
       </c>
@@ -4224,7 +4397,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>31</v>
       </c>
@@ -4245,7 +4418,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>32</v>
       </c>
@@ -4266,7 +4439,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>33</v>
       </c>
@@ -4287,7 +4460,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>34</v>
       </c>
@@ -4308,7 +4481,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>35</v>
       </c>
@@ -4329,7 +4502,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>36</v>
       </c>
@@ -4350,7 +4523,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>37</v>
       </c>
@@ -4372,7 +4545,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>38</v>
       </c>
@@ -4393,7 +4566,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>39</v>
       </c>
@@ -4414,7 +4587,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>40</v>
       </c>
@@ -4435,7 +4608,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>41</v>
       </c>
@@ -4456,7 +4629,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>42</v>
       </c>
@@ -4484,38 +4657,38 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0657A824-9110-B347-821D-B64D54D407AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="7" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="7" max="8" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
       <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="4" t="s">
         <v>16</v>
       </c>
@@ -4523,11 +4696,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -4559,9 +4732,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -4576,7 +4749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>23</v>
       </c>
@@ -4596,7 +4769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>24</v>
       </c>
@@ -4630,7 +4803,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>25</v>
       </c>
@@ -4664,7 +4837,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>26</v>
       </c>
@@ -4705,7 +4878,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>27</v>
       </c>
@@ -4746,7 +4919,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>28</v>
       </c>
@@ -4787,7 +4960,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>29</v>
       </c>
@@ -4828,7 +5001,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>30</v>
       </c>
@@ -4869,7 +5042,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>31</v>
       </c>
@@ -4910,7 +5083,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>32</v>
       </c>
@@ -4951,7 +5124,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>33</v>
       </c>
@@ -4992,7 +5165,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>34</v>
       </c>
@@ -5033,7 +5206,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>35</v>
       </c>
@@ -5074,7 +5247,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>36</v>
       </c>
@@ -5115,7 +5288,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>37</v>
       </c>
@@ -5157,7 +5330,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>38</v>
       </c>
@@ -5198,7 +5371,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>39</v>
       </c>
@@ -5239,7 +5412,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>40</v>
       </c>
@@ -5280,7 +5453,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>41</v>
       </c>
@@ -5321,7 +5494,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Updated scenario 1 test parameter values.
</commit_message>
<xml_diff>
--- a/Scenario 1_test.xlsx
+++ b/Scenario 1_test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdlatour\AppData\Local\Temp\scp29210\local\users\cdlatour\Multiple_outcomes_pregnancy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870CD75B-4AEA-AB41-B577-97FDE80AA1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="825" windowWidth="28800" windowHeight="16215" activeTab="2"/>
+    <workbookView xWindow="28800" yWindow="820" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <sheet name="OLD" sheetId="1" r:id="rId6"/>
     <sheet name="SB_Risk_Preeclampsia" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,26 +42,17 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={2D0EDF39-7EAE-8B42-8A25-E31D9B0584A4}</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0" shapeId="0">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Everyone who has a continuing pregnancy is indexed at week 4. By having more rows, we allow for subsequent simulations where people can be indexed at different gestational weeks.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -68,44 +60,26 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={6F0D0981-BCCC-D340-9528-F44FC96324E0}</author>
     <author>tc={5F2D1E39-8D5C-0A4A-B365-BF113D93EECC}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     DECREASES the risk of fetal death, starting at gestational week 4 from conception (i.e., the week that everyone is indexed into the trial if they have continued their pregnancy.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="1" shapeId="0">
+    <comment ref="D26" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     DECREASES the risk of preterm birth, RR = 0.7, and subsequently increases the risk of term births (&gt;= 35 weeks from conception), RR = 1.05</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -113,82 +87,55 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={64BAD85A-477D-3B47-ACFB-F7563888EB93}</author>
     <author>tc={4842E7A7-EBD7-CE4B-AB5E-5EFBBB07D91E}</author>
     <author>tc={8166E600-F91C-DF49-B3FC-30F8863F4314}</author>
     <author>tc={DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}</author>
+    <author>tc={1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This information is based upon the following. https://www.sciencedirect.com/science/article/pii/S0002937813008594?via%3Dihub#fig1</t>
-        </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1" shapeId="0">
+    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Increased the risk of preeclampsia for the simulation — Individuals with CH are at much higher risk of preeclampsia (e.g., 10-25%) than those without: High blood pressure: A risk factor for preeclampsiaMarch of Dimeshttps://www.marchofdimes.org › find-support › blog › h...</t>
-        </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="2" shapeId="0">
+    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Treatment DECREASES the odds of preeclampsia</t>
-        </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="3" shapeId="0">
+    <comment ref="G1" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/
 Reply:
     Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</t>
-        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="4" shapeId="0" xr:uid="{1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Previously 0.0009</t>
       </text>
     </comment>
   </commentList>
@@ -196,26 +143,17 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={D251C841-2558-B642-82DC-6ED550C61FF7}</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Treatment DECREASES risk of SGA, RR = 0.8</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -223,26 +161,17 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={EB10B5D4-D174-9E46-AE4A-935ECC1C8009}</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Very minimal uninformative censoring.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -250,7 +179,7 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={E6E88FEF-63DE-2F45-80DF-11FAF199CED4}</author>
     <author>tc={B831F326-F008-1346-B1B1-8CC11324C357}</author>
@@ -261,124 +190,61 @@
     <author>tc={922FBB19-8B5B-A34B-A9B0-54F331113989}</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.medicalnewstoday.com/articles/322634#miscarriage-rates-by-week</t>
-        </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Going to assume that once someone develops severe preeclampsia that they </t>
-        </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="2" shapeId="0">
+    <comment ref="B17" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     All the 0.003s — https://stacks.cdc.gov/view/cdc/61387</t>
-        </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="3" shapeId="0">
+    <comment ref="C22" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC9847908/#:~:text=There%20was%20a%20peak%20of,%25)%20occurring%20at%2039%20weeks.</t>
-        </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="4" shapeId="0">
+    <comment ref="E22" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.sciencedirect.com/science/article/pii/S0002937813008594?via%3Dihub#fig1</t>
-        </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="5" shapeId="0">
+    <comment ref="F22" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.cdc.gov/nchs/data/vsrr/vsrr021.pdf
 </t>
-        </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="6" shapeId="0">
+    <comment ref="B33" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -386,63 +252,36 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={7F21C0C9-3748-7449-8B61-7AC75D94AA52}</author>
     <author>tc={760167DC-12EB-F840-B9E8-A3B42A8E8484}</author>
     <author>tc={895E85A6-7599-BE4D-A5A6-2C2F9CEB3D46}</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4347876/#:~:text=However%2C%20relative%20risk%20of%20stillbirth,CI%3D46%20to%20142).</t>
-        </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="1" shapeId="0">
+    <comment ref="L2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The values that going to use, given statistical probs. Assuming that preeclampsia leads to at least as high a probability of fetal death. Going to take the maximimum of the risk here and the risk that we’re using in Phase 1
 </t>
-        </r>
       </text>
     </comment>
-    <comment ref="K18" authorId="2" shapeId="0">
+    <comment ref="K18" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     https://www.ncbi.nlm.nih.gov/pmc/articles/PMC3719843/#:~:text=The%20risk%20of%20stillbirth%20at,at%2042%20weeks%20of%20gestation.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -566,8 +405,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -596,6 +435,19 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -623,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -632,11 +484,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,6 +847,9 @@
   <threadedComment ref="G1" dT="2023-11-25T19:28:53.24" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E6A79F53-3968-FF47-900F-F20537C8C3CA}" parentId="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
     <text>Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</text>
   </threadedComment>
+  <threadedComment ref="B16" dT="2025-02-11T22:41:54.72" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}">
+    <text>Previously 0.0009</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1065,23 +918,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1101,7 +954,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1123,11 +976,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3">
         <f t="shared" ref="B3:B42" si="0">0.5*F3</f>
         <v>0.05</v>
       </c>
@@ -1145,11 +998,11 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1167,11 +1020,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1189,11 +1042,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1211,11 +1064,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1233,11 +1086,11 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1255,11 +1108,11 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1277,11 +1130,11 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1299,11 +1152,11 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1321,11 +1174,11 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1343,11 +1196,11 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
@@ -1365,11 +1218,11 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1387,11 +1240,11 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1409,11 +1262,11 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1431,11 +1284,11 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1453,11 +1306,11 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1475,11 +1328,11 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1497,11 +1350,11 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1519,11 +1372,11 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1541,11 +1394,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1563,11 +1416,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1585,11 +1438,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1607,11 +1460,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1629,11 +1482,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1651,11 +1504,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1673,11 +1526,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1695,11 +1548,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1717,11 +1570,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1739,11 +1592,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1761,11 +1614,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1783,11 +1636,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1805,11 +1658,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1827,11 +1680,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1849,11 +1702,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36">
         <f t="shared" si="0"/>
         <v>1.5E-3</v>
       </c>
@@ -1871,11 +1724,11 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37">
         <f t="shared" si="0"/>
         <v>1.05E-4</v>
       </c>
@@ -1894,11 +1747,11 @@
         <v>2.1000000000000001E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38">
         <f t="shared" si="0"/>
         <v>1.35E-4</v>
       </c>
@@ -1916,11 +1769,11 @@
         <v>2.7E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39">
         <f t="shared" si="0"/>
         <v>1.75E-4</v>
       </c>
@@ -1938,11 +1791,11 @@
         <v>3.5E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40">
         <f t="shared" si="0"/>
         <v>2.1000000000000001E-4</v>
       </c>
@@ -1960,11 +1813,11 @@
         <v>4.2000000000000002E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41">
         <f t="shared" si="0"/>
         <v>3.0499999999999999E-4</v>
       </c>
@@ -1982,11 +1835,11 @@
         <v>6.0999999999999997E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42">
         <f t="shared" si="0"/>
         <v>5.4000000000000001E-4</v>
       </c>
@@ -2011,23 +1864,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.375" customWidth="1"/>
-    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2044,7 +1897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2062,7 +1915,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2080,7 +1933,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2098,7 +1951,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2116,7 +1969,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2135,14 +1988,14 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7">
         <f>0.8*Phase1!B7</f>
         <v>2.0000000000000004E-2</v>
       </c>
@@ -2154,14 +2007,14 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8">
         <f>0.8*Phase1!B8</f>
         <v>1.2E-2</v>
       </c>
@@ -2173,14 +2026,14 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9">
         <f>0.8*Phase1!B9</f>
         <v>1.2E-2</v>
       </c>
@@ -2192,14 +2045,14 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10">
         <f>0.8*Phase1!B10</f>
         <v>1.2E-2</v>
       </c>
@@ -2211,14 +2064,14 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11">
         <f>0.8*Phase1!B11</f>
         <v>1.2E-2</v>
       </c>
@@ -2230,14 +2083,14 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12">
         <f>0.8*Phase1!B12</f>
         <v>1.2E-2</v>
       </c>
@@ -2249,14 +2102,14 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13">
         <f>0.8*Phase1!B13</f>
         <v>1.2E-2</v>
       </c>
@@ -2268,14 +2121,14 @@
         <v>0.98799999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14">
         <f>0.8*Phase1!B14</f>
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2287,14 +2140,14 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15">
         <f>0.8*Phase1!B15</f>
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2306,14 +2159,14 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16">
         <f>0.8*Phase1!B16</f>
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2325,14 +2178,14 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17">
         <f>0.8*Phase1!B17</f>
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2344,14 +2197,14 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18">
         <f>0.8*Phase1!B18</f>
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2363,14 +2216,14 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19">
         <f>0.8*Phase1!B19</f>
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2382,14 +2235,14 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20">
         <f>0.8*Phase1!B20</f>
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2401,14 +2254,14 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21">
         <f>0.8*Phase1!B21</f>
         <v>1.2000000000000001E-3</v>
       </c>
@@ -2420,14 +2273,14 @@
         <v>0.99880000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22">
         <f>0.8*Phase1!B22</f>
         <v>1.2000000000000001E-3</v>
       </c>
@@ -2439,14 +2292,14 @@
         <v>0.99880000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23">
         <f>0.8*Phase1!B23</f>
         <v>1.2000000000000001E-3</v>
       </c>
@@ -2458,14 +2311,14 @@
         <v>0.99880000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24">
         <f>0.8*Phase1!B24</f>
         <v>1.2000000000000001E-3</v>
       </c>
@@ -2477,14 +2330,14 @@
         <v>0.99880000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25">
         <f>0.8*Phase1!B25</f>
         <v>1.2000000000000001E-3</v>
       </c>
@@ -2496,14 +2349,14 @@
         <v>0.99880000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26">
         <f>0.8*Phase1!B26</f>
         <v>1.2000000000000001E-3</v>
       </c>
@@ -2516,18 +2369,18 @@
         <v>0.99080000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27">
         <f>0.8*Phase1!B27</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27">
         <f>0.8*Phase1!C27</f>
         <v>8.0000000000000002E-3</v>
       </c>
@@ -2536,18 +2389,18 @@
         <v>0.99080000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28">
         <f>0.8*Phase1!B28</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28">
         <f>0.8*Phase1!C28</f>
         <v>1.2E-2</v>
       </c>
@@ -2556,18 +2409,18 @@
         <v>0.98680000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29">
         <f>0.8*Phase1!B29</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29">
         <f>0.8*Phase1!C29</f>
         <v>1.2E-2</v>
       </c>
@@ -2576,18 +2429,18 @@
         <v>0.98680000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30">
         <f>0.8*Phase1!B30</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30">
         <f>0.8*Phase1!C30</f>
         <v>1.6E-2</v>
       </c>
@@ -2596,18 +2449,18 @@
         <v>0.98280000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31">
         <f>0.8*Phase1!B31</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31">
         <f>0.8*Phase1!C31</f>
         <v>1.6E-2</v>
       </c>
@@ -2616,18 +2469,18 @@
         <v>0.98280000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32">
         <f>0.8*Phase1!B32</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32">
         <f>0.8*Phase1!C32</f>
         <v>2.0000000000000004E-2</v>
       </c>
@@ -2636,18 +2489,18 @@
         <v>0.9788</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33">
         <f>0.8*Phase1!B33</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33">
         <f>0.8*Phase1!C33</f>
         <v>2.4E-2</v>
       </c>
@@ -2656,18 +2509,18 @@
         <v>0.9748</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34">
         <f>0.8*Phase1!B34</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34">
         <f>0.8*Phase1!C34</f>
         <v>7.1999999999999995E-2</v>
       </c>
@@ -2676,18 +2529,18 @@
         <v>0.92680000000000007</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35">
         <f>0.8*Phase1!B35</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35">
         <f>0.8*Phase1!C35</f>
         <v>7.1999999999999995E-2</v>
       </c>
@@ -2696,18 +2549,18 @@
         <v>0.92680000000000007</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36">
         <f>0.8*Phase1!B36</f>
         <v>1.2000000000000001E-3</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36">
         <f>0.8*Phase1!C36</f>
         <v>7.1999999999999995E-2</v>
       </c>
@@ -2716,14 +2569,14 @@
         <v>0.92680000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37">
         <f>0.8*Phase1!B37</f>
         <v>8.4000000000000009E-5</v>
       </c>
@@ -2736,14 +2589,14 @@
         <v>0.68491600000000008</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38">
         <f>0.8*Phase1!B38</f>
         <v>1.0800000000000001E-4</v>
       </c>
@@ -2756,14 +2609,14 @@
         <v>0.63239200000000007</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39">
         <f>0.8*Phase1!B39</f>
         <v>1.4000000000000001E-4</v>
       </c>
@@ -2776,14 +2629,14 @@
         <v>0.26485999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40">
         <f>0.8*Phase1!B40</f>
         <v>1.6800000000000002E-4</v>
       </c>
@@ -2796,14 +2649,14 @@
         <v>0.26483200000000007</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41">
         <f>0.8*Phase1!B41</f>
         <v>2.4399999999999999E-4</v>
       </c>
@@ -2816,14 +2669,14 @@
         <v>0.26475599999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42">
         <f>0.8*Phase1!B42</f>
         <v>4.3200000000000004E-4</v>
       </c>
@@ -2842,26 +2695,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
-    <col min="4" max="4" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.125" customWidth="1"/>
-    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2887,7 +2740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>24</v>
       </c>
@@ -2895,12 +2748,12 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C2">
-        <f>16*B2</f>
-        <v>6.4000000000000003E-3</v>
+        <f>19*B2</f>
+        <v>7.6E-3</v>
       </c>
       <c r="D2">
         <f>LN(C2/(1-C2))</f>
-        <v>-5.045036720813588</v>
+        <v>-4.8719780045253609</v>
       </c>
       <c r="E2">
         <v>0.6</v>
@@ -2917,22 +2770,22 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>25</v>
       </c>
       <c r="B3">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="C3" s="8">
-        <f t="shared" ref="C3:C18" si="1">16*B3</f>
-        <v>6.4000000000000003E-3</v>
+      <c r="C3">
+        <f t="shared" ref="C3:C18" si="1">20*B3</f>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D3">
         <f>LN(C3/(1-C3))</f>
-        <v>-5.045036720813588</v>
-      </c>
-      <c r="E3" s="7">
+        <v>-4.8202815656050371</v>
+      </c>
+      <c r="E3">
         <v>0.6</v>
       </c>
       <c r="F3">
@@ -2947,22 +2800,22 @@
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>26</v>
       </c>
       <c r="B4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="C4" s="8">
-        <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D18" si="2">LN(C4/(1-C4))</f>
-        <v>-4.8202815656050371</v>
-      </c>
-      <c r="E4" s="7">
+        <v>-4.5951198501345898</v>
+      </c>
+      <c r="E4">
         <v>0.6</v>
       </c>
       <c r="F4">
@@ -2977,22 +2830,22 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>27</v>
       </c>
       <c r="B5">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="C5" s="8">
-        <f t="shared" si="1"/>
-        <v>9.5999999999999992E-3</v>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>1.1999999999999999E-2</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>-4.6363458034565408</v>
-      </c>
-      <c r="E5" s="7">
+        <v>-4.4107760479598674</v>
+      </c>
+      <c r="E5">
         <v>0.6</v>
       </c>
       <c r="F5">
@@ -3007,22 +2860,22 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>28</v>
       </c>
       <c r="B6">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="C6" s="8">
-        <f t="shared" si="1"/>
-        <v>1.12E-2</v>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1.4E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>-4.4805783084023778</v>
-      </c>
-      <c r="E6" s="7">
+        <v>-4.2545990249873764</v>
+      </c>
+      <c r="E6">
         <v>0.6</v>
       </c>
       <c r="F6">
@@ -3037,22 +2890,22 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>29</v>
       </c>
       <c r="B7">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="C7" s="8">
-        <f t="shared" si="1"/>
-        <v>1.2800000000000001E-2</v>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>1.6E-2</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>-4.3454274822255519</v>
-      </c>
-      <c r="E7" s="7">
+        <v>-4.1190371748124717</v>
+      </c>
+      <c r="E7">
         <v>0.6</v>
       </c>
       <c r="F7">
@@ -3067,22 +2920,22 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>30</v>
       </c>
       <c r="B8">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="C8" s="8">
-        <f t="shared" si="1"/>
-        <v>1.44E-2</v>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>-4.2260223861973003</v>
-      </c>
-      <c r="E8" s="7">
+        <v>-3.9992195504583012</v>
+      </c>
+      <c r="E8">
         <v>0.6</v>
       </c>
       <c r="F8">
@@ -3097,22 +2950,22 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>31</v>
       </c>
       <c r="B9">
         <v>1E-3</v>
       </c>
-      <c r="C9" s="8">
-        <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>-4.1190371748124717</v>
-      </c>
-      <c r="E9" s="7">
+        <v>-3.8918202981106265</v>
+      </c>
+      <c r="E9">
         <v>0.6</v>
       </c>
       <c r="F9">
@@ -3127,22 +2980,22 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>32</v>
       </c>
       <c r="B10">
         <v>1.8E-3</v>
       </c>
-      <c r="C10" s="8">
-        <f t="shared" si="1"/>
-        <v>2.8799999999999999E-2</v>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>-3.5181570331633334</v>
-      </c>
-      <c r="E10" s="7">
+        <v>-3.2875723561544357</v>
+      </c>
+      <c r="E10">
         <v>0.6</v>
       </c>
       <c r="F10">
@@ -3157,22 +3010,22 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>33</v>
       </c>
       <c r="B11">
         <v>2E-3</v>
       </c>
-      <c r="C11" s="8">
-        <f t="shared" si="1"/>
-        <v>3.2000000000000001E-2</v>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>-3.4094961844768505</v>
-      </c>
-      <c r="E11" s="7">
+        <v>-3.1780538303479453</v>
+      </c>
+      <c r="E11">
         <v>0.6</v>
       </c>
       <c r="F11">
@@ -3187,22 +3040,22 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>34</v>
       </c>
       <c r="B12">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="C12" s="8">
-        <f t="shared" si="1"/>
-        <v>6.4000000000000001E-2</v>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>-2.6827323931179201</v>
-      </c>
-      <c r="E12" s="7">
+        <v>-2.4423470353692043</v>
+      </c>
+      <c r="E12">
         <v>0.6</v>
       </c>
       <c r="F12">
@@ -3217,22 +3070,22 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>35</v>
       </c>
       <c r="B13">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C13" s="8">
-        <f t="shared" si="1"/>
-        <v>0.08</v>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>-2.4423470353692043</v>
-      </c>
-      <c r="E13" s="7">
+        <v>-2.1972245773362191</v>
+      </c>
+      <c r="E13">
         <v>0.6</v>
       </c>
       <c r="F13">
@@ -3247,22 +3100,22 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>36</v>
       </c>
       <c r="B14">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C14" s="8">
-        <f t="shared" si="1"/>
-        <v>0.112</v>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>-2.0704728716970755</v>
-      </c>
-      <c r="E14" s="7">
+        <v>-1.8152899666382492</v>
+      </c>
+      <c r="E14">
         <v>0.6</v>
       </c>
       <c r="F14">
@@ -3277,22 +3130,22 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>37</v>
       </c>
       <c r="B15">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C15" s="8">
-        <f t="shared" si="1"/>
-        <v>0.128</v>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.16</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>-1.9187591599893623</v>
-      </c>
-      <c r="E15" s="7">
+        <v>-1.6582280766035322</v>
+      </c>
+      <c r="E15">
         <v>0.6</v>
       </c>
       <c r="F15">
@@ -3307,22 +3160,22 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>38</v>
       </c>
-      <c r="B16">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="C16" s="8">
-        <f t="shared" si="1"/>
-        <v>1.44E-2</v>
+      <c r="B16" s="8">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>-4.2260223861973003</v>
-      </c>
-      <c r="E16" s="7">
+        <v>-1.5163474893680886</v>
+      </c>
+      <c r="E16">
         <v>0.6</v>
       </c>
       <c r="F16">
@@ -3337,22 +3190,22 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>39</v>
       </c>
       <c r="B17">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="C17" s="8">
-        <f t="shared" si="1"/>
-        <v>0.17599999999999999</v>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.21999999999999997</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>-1.54368653487132</v>
-      </c>
-      <c r="E17" s="7">
+        <v>-1.2656663733312761</v>
+      </c>
+      <c r="E17">
         <v>0.6</v>
       </c>
       <c r="F17">
@@ -3367,22 +3220,22 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>40</v>
       </c>
       <c r="B18">
         <v>1.4E-2</v>
       </c>
-      <c r="C18" s="8">
-        <f t="shared" si="1"/>
-        <v>0.224</v>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>-1.242506468328179</v>
-      </c>
-      <c r="E18" s="7">
+        <v>-0.94446160884085117</v>
+      </c>
+      <c r="E18">
         <v>0.6</v>
       </c>
       <c r="F18">
@@ -3404,20 +3257,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
@@ -3428,7 +3281,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3439,7 +3292,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3451,7 +3304,7 @@
         <v>0.15625</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3463,7 +3316,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3482,20 +3335,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -3503,7 +3356,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3511,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3519,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3527,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3535,7 +3388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3543,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3551,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3559,275 +3412,275 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -3838,21 +3691,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22:E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3872,7 +3725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>6</v>
       </c>
@@ -3893,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>7</v>
       </c>
@@ -3914,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8</v>
       </c>
@@ -3935,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9</v>
       </c>
@@ -3956,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
@@ -3977,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>11</v>
       </c>
@@ -3998,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>12</v>
       </c>
@@ -4019,7 +3872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>13</v>
       </c>
@@ -4040,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>14</v>
       </c>
@@ -4061,7 +3914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>15</v>
       </c>
@@ -4082,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>16</v>
       </c>
@@ -4103,7 +3956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>17</v>
       </c>
@@ -4124,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>18</v>
       </c>
@@ -4145,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>19</v>
       </c>
@@ -4166,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20</v>
       </c>
@@ -4187,7 +4040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>21</v>
       </c>
@@ -4208,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>22</v>
       </c>
@@ -4229,7 +4082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>23</v>
       </c>
@@ -4250,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>24</v>
       </c>
@@ -4271,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>25</v>
       </c>
@@ -4292,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>26</v>
       </c>
@@ -4313,7 +4166,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>27</v>
       </c>
@@ -4334,7 +4187,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>28</v>
       </c>
@@ -4355,7 +4208,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>29</v>
       </c>
@@ -4376,7 +4229,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>30</v>
       </c>
@@ -4397,7 +4250,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>31</v>
       </c>
@@ -4418,7 +4271,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>32</v>
       </c>
@@ -4439,7 +4292,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>33</v>
       </c>
@@ -4460,7 +4313,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>34</v>
       </c>
@@ -4481,7 +4334,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>35</v>
       </c>
@@ -4502,7 +4355,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>36</v>
       </c>
@@ -4523,7 +4376,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>37</v>
       </c>
@@ -4545,7 +4398,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>38</v>
       </c>
@@ -4566,7 +4419,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>39</v>
       </c>
@@ -4587,7 +4440,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>40</v>
       </c>
@@ -4608,7 +4461,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>41</v>
       </c>
@@ -4629,7 +4482,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>42</v>
       </c>
@@ -4657,38 +4510,38 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="7" max="8" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="7" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="4" t="s">
         <v>16</v>
       </c>
@@ -4696,11 +4549,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -4732,9 +4585,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -4749,7 +4602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>23</v>
       </c>
@@ -4769,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>24</v>
       </c>
@@ -4803,7 +4656,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>25</v>
       </c>
@@ -4837,7 +4690,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>26</v>
       </c>
@@ -4878,7 +4731,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>27</v>
       </c>
@@ -4919,7 +4772,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>28</v>
       </c>
@@ -4960,7 +4813,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>29</v>
       </c>
@@ -5001,7 +4854,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>30</v>
       </c>
@@ -5042,7 +4895,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>31</v>
       </c>
@@ -5083,7 +4936,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>32</v>
       </c>
@@ -5124,7 +4977,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>33</v>
       </c>
@@ -5165,7 +5018,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>34</v>
       </c>
@@ -5206,7 +5059,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>35</v>
       </c>
@@ -5247,7 +5100,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>36</v>
       </c>
@@ -5288,7 +5141,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>37</v>
       </c>
@@ -5330,7 +5183,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>38</v>
       </c>
@@ -5371,7 +5224,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>39</v>
       </c>
@@ -5412,7 +5265,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>40</v>
       </c>
@@ -5453,7 +5306,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>41</v>
       </c>
@@ -5494,7 +5347,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Updating the testing values.
</commit_message>
<xml_diff>
--- a/Scenario 1_test.xlsx
+++ b/Scenario 1_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0007A77B-E15B-4445-8CD0-7471694CFDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330DB184-BBF1-7E4C-AA20-E325E52756E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="820" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2698,7 +2698,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2755,11 +2755,11 @@
         <v>-5.1099777374285189</v>
       </c>
       <c r="E2">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F2">
         <f>LN(E2)</f>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G2">
         <v>1.7000000000000001E-2</v>
@@ -2785,11 +2785,11 @@
         <v>-5.1099777374285189</v>
       </c>
       <c r="E3">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F3">
         <f>LN(E3)</f>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G3">
         <v>1.7000000000000001E-2</v>
@@ -2815,11 +2815,11 @@
         <v>-4.8853239920190807</v>
       </c>
       <c r="E4">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F18" si="3">LN(E4)</f>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G4">
         <v>3.0000000000000001E-3</v>
@@ -2845,11 +2845,11 @@
         <v>-4.7014899569937691</v>
       </c>
       <c r="E5">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G5">
         <v>4.0000000000000001E-3</v>
@@ -2875,11 +2875,11 @@
         <v>-4.5458245078791428</v>
       </c>
       <c r="E6">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G6">
         <v>3.0000000000000001E-3</v>
@@ -2905,11 +2905,11 @@
         <v>-4.4107760479598674</v>
       </c>
       <c r="E7">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G7">
         <v>3.0000000000000001E-3</v>
@@ -2935,11 +2935,11 @@
         <v>-4.2914736400182862</v>
       </c>
       <c r="E8">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G8">
         <v>3.0000000000000001E-3</v>
@@ -2965,11 +2965,11 @@
         <v>-4.1845914400698785</v>
       </c>
       <c r="E9">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G9">
         <v>3.0000000000000001E-3</v>
@@ -2995,11 +2995,11 @@
         <v>-3.1421930058942622</v>
       </c>
       <c r="E10">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G10">
         <v>3.0000000000000001E-3</v>
@@ -3025,11 +3025,11 @@
         <v>-3.0320222749591914</v>
       </c>
       <c r="E11">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G11">
         <v>3.0000000000000001E-3</v>
@@ -3055,11 +3055,11 @@
         <v>-2.2894558015522528</v>
       </c>
       <c r="E12">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G12">
         <v>3.0000000000000001E-3</v>
@@ -3085,11 +3085,11 @@
         <v>-2.0406555166446796</v>
       </c>
       <c r="E13">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G13">
         <v>1E-3</v>
@@ -3115,11 +3115,11 @@
         <v>-1.6508063414827432</v>
       </c>
       <c r="E14">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G14">
         <v>1E-3</v>
@@ -3145,11 +3145,11 @@
         <v>-1.4894785973551214</v>
       </c>
       <c r="E15">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G15">
         <v>1E-3</v>
@@ -3175,11 +3175,11 @@
         <v>-1.3431044283694791</v>
       </c>
       <c r="E16">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G16">
         <v>1E-3</v>
@@ -3205,11 +3205,11 @@
         <v>-1.082675696405297</v>
       </c>
       <c r="E17">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G17">
         <v>2E-3</v>
@@ -3235,11 +3235,11 @@
         <v>-0.74459574239598714</v>
       </c>
       <c r="E18">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
-        <v>-0.51082562376599072</v>
+        <v>-0.2876820724517809</v>
       </c>
       <c r="G18">
         <v>1E-3</v>
@@ -5400,15 +5400,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -5633,15 +5624,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5658,4 +5650,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
New testing values for scenario 1
</commit_message>
<xml_diff>
--- a/Scenario 1_test.xlsx
+++ b/Scenario 1_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312612D3-A7B7-A540-AC20-A497912A21CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D674F55A-1B3B-1243-BAB6-2A5231C8D950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="820" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="820" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -129,6 +129,8 @@
     <author>tc={4842E7A7-EBD7-CE4B-AB5E-5EFBBB07D91E}</author>
     <author>tc={8166E600-F91C-DF49-B3FC-30F8863F4314}</author>
     <author>tc={DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}</author>
+    <author>tc={90C4F836-EECA-6C42-BA76-A91238556A97}</author>
+    <author>tc={B86182D7-D97A-584B-B468-910341D49944}</author>
     <author>tc={1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}</author>
   </authors>
   <commentList>
@@ -168,7 +170,23 @@
     Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</t>
       </text>
     </comment>
-    <comment ref="B16" authorId="4" shapeId="0" xr:uid="{1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}">
+    <comment ref="B14" authorId="4" shapeId="0" xr:uid="{90C4F836-EECA-6C42-BA76-A91238556A97}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally 0.007. Bumped up to 0.01</t>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="5" shapeId="0" xr:uid="{B86182D7-D97A-584B-B468-910341D49944}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally 0.008. Bumped up to 0.01</t>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="6" shapeId="0" xr:uid="{1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -900,6 +918,12 @@
   <threadedComment ref="G1" dT="2023-11-25T19:28:53.24" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E6A79F53-3968-FF47-900F-F20537C8C3CA}" parentId="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
     <text>Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</text>
   </threadedComment>
+  <threadedComment ref="B14" dT="2025-02-13T16:48:00.34" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{90C4F836-EECA-6C42-BA76-A91238556A97}">
+    <text>Originally 0.007. Bumped up to 0.01</text>
+  </threadedComment>
+  <threadedComment ref="B15" dT="2025-02-13T16:48:00.34" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{B86182D7-D97A-584B-B468-910341D49944}">
+    <text>Originally 0.008. Bumped up to 0.01</text>
+  </threadedComment>
   <threadedComment ref="B16" dT="2025-02-11T22:41:54.72" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}">
     <text>Previously 0.0009</text>
   </threadedComment>
@@ -974,7 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -2751,8 +2775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2809,11 +2833,11 @@
         <v>-5.1099777374285189</v>
       </c>
       <c r="E2">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F2">
         <f>LN(E2)</f>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G2">
         <v>1.7000000000000001E-2</v>
@@ -2839,11 +2863,11 @@
         <v>-5.1099777374285189</v>
       </c>
       <c r="E3">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F3">
         <f>LN(E3)</f>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G3">
         <v>1.7000000000000001E-2</v>
@@ -2869,11 +2893,11 @@
         <v>-4.8853239920190807</v>
       </c>
       <c r="E4">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F18" si="3">LN(E4)</f>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G4">
         <v>3.0000000000000001E-3</v>
@@ -2899,11 +2923,11 @@
         <v>-4.7014899569937691</v>
       </c>
       <c r="E5">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G5">
         <v>4.0000000000000001E-3</v>
@@ -2929,11 +2953,11 @@
         <v>-4.5458245078791428</v>
       </c>
       <c r="E6">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G6">
         <v>3.0000000000000001E-3</v>
@@ -2959,11 +2983,11 @@
         <v>-4.4107760479598674</v>
       </c>
       <c r="E7">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G7">
         <v>3.0000000000000001E-3</v>
@@ -2981,19 +3005,19 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>1.35E-2</v>
+        <f>18*B8</f>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>-4.2914736400182862</v>
+        <v>-4.1064113821229009</v>
       </c>
       <c r="E8">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G8">
         <v>3.0000000000000001E-3</v>
@@ -3011,19 +3035,19 @@
         <v>1E-3</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <f>18*B9</f>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>-4.1845914400698785</v>
+        <v>-3.9992195504583012</v>
       </c>
       <c r="E9">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G9">
         <v>3.0000000000000001E-3</v>
@@ -3041,19 +3065,19 @@
         <v>1.8E-3</v>
       </c>
       <c r="C10">
-        <f>25*B10</f>
-        <v>4.4999999999999998E-2</v>
+        <f>26*B10</f>
+        <v>4.6800000000000001E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>-3.0550488507104103</v>
+        <v>-3.0139415423009859</v>
       </c>
       <c r="E10">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G10">
         <v>3.0000000000000001E-3</v>
@@ -3071,19 +3095,19 @@
         <v>2E-3</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C18" si="4">25*B11</f>
-        <v>0.05</v>
+        <f t="shared" ref="C11:C18" si="4">26*B11</f>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>-2.9444389791664403</v>
+        <v>-2.9031107836735943</v>
       </c>
       <c r="E11">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G11">
         <v>3.0000000000000001E-3</v>
@@ -3102,18 +3126,18 @@
       </c>
       <c r="C12">
         <f t="shared" si="4"/>
-        <v>0.1</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>-2.1972245773362191</v>
+        <v>-2.1535495138335579</v>
       </c>
       <c r="E12">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G12">
         <v>3.0000000000000001E-3</v>
@@ -3132,18 +3156,18 @@
       </c>
       <c r="C13">
         <f t="shared" si="4"/>
-        <v>0.125</v>
+        <v>0.13</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>-1.9459101490553135</v>
+        <v>-1.900958761193047</v>
       </c>
       <c r="E13">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G13">
         <v>1E-3</v>
@@ -3157,23 +3181,23 @@
       <c r="A14">
         <v>36</v>
       </c>
-      <c r="B14">
-        <v>7.0000000000000001E-3</v>
+      <c r="B14" s="6">
+        <v>0.01</v>
       </c>
       <c r="C14">
         <f t="shared" si="4"/>
-        <v>0.17500000000000002</v>
+        <v>0.26</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>-1.5505974124111668</v>
+        <v>-1.0459685551826876</v>
       </c>
       <c r="E14">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G14">
         <v>1E-3</v>
@@ -3187,23 +3211,23 @@
       <c r="A15">
         <v>37</v>
       </c>
-      <c r="B15">
-        <v>8.0000000000000002E-3</v>
+      <c r="B15" s="6">
+        <v>0.01</v>
       </c>
       <c r="C15">
         <f t="shared" si="4"/>
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>-1.3862943611198906</v>
+        <v>-1.0459685551826876</v>
       </c>
       <c r="E15">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G15">
         <v>1E-3</v>
@@ -3218,22 +3242,22 @@
         <v>38</v>
       </c>
       <c r="B16" s="6">
-        <v>8.9999999999999993E-3</v>
+        <v>0.01</v>
       </c>
       <c r="C16">
         <f t="shared" si="4"/>
-        <v>0.22499999999999998</v>
+        <v>0.26</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>-1.2367626271489269</v>
+        <v>-1.0459685551826876</v>
       </c>
       <c r="E16">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G16">
         <v>1E-3</v>
@@ -3252,18 +3276,18 @@
       </c>
       <c r="C17">
         <f t="shared" si="4"/>
-        <v>0.27499999999999997</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>-0.9694005571881037</v>
+        <v>-0.91489115151973188</v>
       </c>
       <c r="E17">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G17">
         <v>2E-3</v>
@@ -3282,18 +3306,18 @@
       </c>
       <c r="C18">
         <f t="shared" si="4"/>
-        <v>0.35000000000000003</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>-0.61903920840622328</v>
+        <v>-0.55804469570338155</v>
       </c>
       <c r="E18">
-        <v>0.75</v>
+        <v>0.65</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.43078291609245423</v>
       </c>
       <c r="G18">
         <v>1E-3</v>

</xml_diff>

<commit_message>
Uploading new test values.
</commit_message>
<xml_diff>
--- a/Scenario 1_test.xlsx
+++ b/Scenario 1_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1404CB23-F8EE-3746-BD9B-F67DB6E20FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9355EE-E5A3-B24D-BE77-CC033CEABB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="820" windowWidth="28800" windowHeight="16220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2770,7 +2770,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2977,11 +2977,11 @@
         <v>-4.4107760479598674</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>-0.69314718055994529</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G7">
         <v>3.0000000000000001E-3</v>
@@ -3007,11 +3007,11 @@
         <v>-4.1064113821229009</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>-0.69314718055994529</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G8">
         <v>3.0000000000000001E-3</v>
@@ -3037,11 +3037,11 @@
         <v>-3.9992195504583012</v>
       </c>
       <c r="E9">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>-0.69314718055994529</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G9">
         <v>3.0000000000000001E-3</v>
@@ -3067,11 +3067,11 @@
         <v>-3.0139415423009859</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>-0.69314718055994529</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G10">
         <v>3.0000000000000001E-3</v>
@@ -3097,11 +3097,11 @@
         <v>-2.9031107836735943</v>
       </c>
       <c r="E11">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>-0.22314355131420971</v>
+        <v>-0.35667494393873245</v>
       </c>
       <c r="G11">
         <v>3.0000000000000001E-3</v>
@@ -3127,11 +3127,11 @@
         <v>-2.1535495138335579</v>
       </c>
       <c r="E12">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>-0.22314355131420971</v>
+        <v>-0.35667494393873245</v>
       </c>
       <c r="G12">
         <v>3.0000000000000001E-3</v>
@@ -3157,11 +3157,11 @@
         <v>-1.900958761193047</v>
       </c>
       <c r="E13">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>-0.22314355131420971</v>
+        <v>-0.35667494393873245</v>
       </c>
       <c r="G13">
         <v>1E-3</v>
@@ -3187,11 +3187,11 @@
         <v>-1.0459685551826876</v>
       </c>
       <c r="E14">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>-0.22314355131420971</v>
+        <v>-0.35667494393873245</v>
       </c>
       <c r="G14">
         <v>1E-3</v>

</xml_diff>

<commit_message>
Updating data generation parameters for all scenarios. Further, indexing individuals into the cohort later in gestation.
</commit_message>
<xml_diff>
--- a/Scenario 1_test.xlsx
+++ b/Scenario 1_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312612D3-A7B7-A540-AC20-A497912A21CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B65BDF-E31F-984B-A979-046DB8E13FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="820" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -129,6 +129,8 @@
     <author>tc={4842E7A7-EBD7-CE4B-AB5E-5EFBBB07D91E}</author>
     <author>tc={8166E600-F91C-DF49-B3FC-30F8863F4314}</author>
     <author>tc={DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}</author>
+    <author>tc={90C4F836-EECA-6C42-BA76-A91238556A97}</author>
+    <author>tc={B86182D7-D97A-584B-B468-910341D49944}</author>
     <author>tc={1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}</author>
   </authors>
   <commentList>
@@ -168,7 +170,23 @@
     Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</t>
       </text>
     </comment>
-    <comment ref="B16" authorId="4" shapeId="0" xr:uid="{1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}">
+    <comment ref="B14" authorId="4" shapeId="0" xr:uid="{90C4F836-EECA-6C42-BA76-A91238556A97}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally 0.007. Bumped up to 0.01</t>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="5" shapeId="0" xr:uid="{B86182D7-D97A-584B-B468-910341D49944}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally 0.008. Bumped up to 0.01</t>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="6" shapeId="0" xr:uid="{1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -444,7 +462,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -479,12 +497,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -900,6 +912,12 @@
   <threadedComment ref="G1" dT="2023-11-25T19:28:53.24" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{E6A79F53-3968-FF47-900F-F20537C8C3CA}" parentId="{DC70E6C4-DF0E-954B-B2D1-90B51812DBEA}">
     <text>Note that we have no treatment effect on risk of fetal death or live birth after preeclampsia. We’re assuming that this effect is essentially totally determined by the experience of preeclampsia. This is a simplification of real life.</text>
   </threadedComment>
+  <threadedComment ref="B14" dT="2025-02-13T16:48:00.34" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{90C4F836-EECA-6C42-BA76-A91238556A97}">
+    <text>Originally 0.007. Bumped up to 0.01</text>
+  </threadedComment>
+  <threadedComment ref="B15" dT="2025-02-13T16:48:00.34" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{B86182D7-D97A-584B-B468-910341D49944}">
+    <text>Originally 0.008. Bumped up to 0.01</text>
+  </threadedComment>
   <threadedComment ref="B16" dT="2025-02-11T22:41:54.72" personId="{51D2B8DB-A2F5-4646-800E-4DB3664DB2F8}" id="{1E7A42DE-7A0A-1A48-A5F2-009B8D95C91D}">
     <text>Previously 0.0009</text>
   </threadedComment>
@@ -974,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1920,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A20" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2182,15 +2200,15 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <f>0.8*Phase1!B14</f>
-        <v>4.0000000000000001E-3</v>
+        <f>0.5*Phase1!B14</f>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>0.996</v>
+        <v>0.99750000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2201,15 +2219,15 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <f>0.8*Phase1!B15</f>
-        <v>4.0000000000000001E-3</v>
+        <f>0.5*Phase1!B15</f>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>0.996</v>
+        <v>0.99750000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2220,15 +2238,15 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <f>0.8*Phase1!B16</f>
-        <v>4.0000000000000001E-3</v>
+        <f>0.5*Phase1!B16</f>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>0.996</v>
+        <v>0.99750000000000005</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2239,15 +2257,15 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <f>0.8*Phase1!B17</f>
-        <v>4.0000000000000001E-3</v>
+        <f>0.5*Phase1!B17</f>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>0.996</v>
+        <v>0.99750000000000005</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2258,15 +2276,15 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <f>0.8*Phase1!B18</f>
-        <v>4.0000000000000001E-3</v>
+        <f>0.5*Phase1!B18</f>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
-        <v>0.996</v>
+        <v>0.99750000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2277,15 +2295,15 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <f>0.8*Phase1!B19</f>
-        <v>4.0000000000000001E-3</v>
+        <f>0.6*Phase1!B19</f>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>0.996</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2296,15 +2314,15 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <f>0.8*Phase1!B20</f>
-        <v>4.0000000000000001E-3</v>
+        <f>0.6*Phase1!B20</f>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>0.996</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2315,15 +2333,15 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <f>0.8*Phase1!B21</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.6*Phase1!B21</f>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>0.99880000000000002</v>
+        <v>0.99909999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2334,15 +2352,15 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <f>0.8*Phase1!B22</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.6*Phase1!B22</f>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
-        <v>0.99880000000000002</v>
+        <v>0.99909999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2353,15 +2371,15 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <f>0.8*Phase1!B23</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.6*Phase1!B23</f>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>0.99880000000000002</v>
+        <v>0.99909999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2372,15 +2390,15 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <f>0.8*Phase1!B24</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.6*Phase1!B24</f>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>0.99880000000000002</v>
+        <v>0.99909999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2391,15 +2409,15 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <f>0.8*Phase1!B25</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.7*Phase1!B25</f>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>0.99880000000000002</v>
+        <v>0.99895</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2410,16 +2428,16 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <f>0.8*Phase1!B26</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.7*Phase1!B26</f>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="D26">
-        <f>0.8*Phase1!C26</f>
-        <v>8.0000000000000002E-3</v>
+        <f>0.6*Phase1!C26</f>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
-        <v>0.99080000000000001</v>
+        <v>0.99295</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2430,16 +2448,16 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <f>0.8*Phase1!B27</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.7*Phase1!B27</f>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="D27">
-        <f>0.8*Phase1!C27</f>
-        <v>8.0000000000000002E-3</v>
+        <f>0.6*Phase1!C27</f>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E27">
         <f t="shared" si="2"/>
-        <v>0.99080000000000001</v>
+        <v>0.99295</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2450,16 +2468,16 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <f>0.8*Phase1!B28</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.7*Phase1!B28</f>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="D28">
-        <f>0.8*Phase1!C28</f>
-        <v>1.2E-2</v>
+        <f>0.6*Phase1!C28</f>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E28">
         <f t="shared" si="2"/>
-        <v>0.98680000000000001</v>
+        <v>0.98995</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2470,16 +2488,16 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <f>0.8*Phase1!B29</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.7*Phase1!B29</f>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="D29">
-        <f>0.8*Phase1!C29</f>
-        <v>1.2E-2</v>
+        <f>0.6*Phase1!C29</f>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E29">
         <f t="shared" si="2"/>
-        <v>0.98680000000000001</v>
+        <v>0.98995</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2490,16 +2508,16 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <f>0.8*Phase1!B30</f>
-        <v>1.2000000000000001E-3</v>
+        <f>0.7*Phase1!B30</f>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="D30">
-        <f>0.8*Phase1!C30</f>
-        <v>1.6E-2</v>
+        <f>0.7*Phase1!C30</f>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
-        <v>0.98280000000000001</v>
+        <v>0.98494999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2514,12 +2532,12 @@
         <v>1.2000000000000001E-3</v>
       </c>
       <c r="D31">
-        <f>0.8*Phase1!C31</f>
-        <v>1.6E-2</v>
+        <f>0.7*Phase1!C31</f>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="E31">
         <f t="shared" si="2"/>
-        <v>0.98280000000000001</v>
+        <v>0.98480000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2534,12 +2552,12 @@
         <v>1.2000000000000001E-3</v>
       </c>
       <c r="D32">
-        <f>0.8*Phase1!C32</f>
-        <v>2.0000000000000004E-2</v>
+        <f>0.7*Phase1!C32</f>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="E32">
         <f t="shared" si="2"/>
-        <v>0.9788</v>
+        <v>0.98130000000000006</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -2554,12 +2572,12 @@
         <v>1.2000000000000001E-3</v>
       </c>
       <c r="D33">
-        <f>0.8*Phase1!C33</f>
-        <v>4.8000000000000001E-2</v>
+        <f>0.7*Phase1!C33</f>
+        <v>4.1999999999999996E-2</v>
       </c>
       <c r="E33">
         <f t="shared" si="2"/>
-        <v>0.95079999999999998</v>
+        <v>0.95679999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2630,8 +2648,8 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <f>0.8*Phase1!B37</f>
-        <v>8.4000000000000009E-5</v>
+        <f>0.9*Phase1!B37</f>
+        <v>9.4500000000000007E-5</v>
       </c>
       <c r="D37">
         <f>1.05*Phase1!C37</f>
@@ -2639,7 +2657,7 @@
       </c>
       <c r="E37">
         <f t="shared" si="2"/>
-        <v>0.68491600000000008</v>
+        <v>0.68490549999999994</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2650,8 +2668,8 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <f>0.8*Phase1!B38</f>
-        <v>1.0800000000000001E-4</v>
+        <f>0.9*Phase1!B38</f>
+        <v>1.215E-4</v>
       </c>
       <c r="D38">
         <f>1.05*Phase1!C38</f>
@@ -2659,7 +2677,7 @@
       </c>
       <c r="E38">
         <f t="shared" si="2"/>
-        <v>0.63239200000000007</v>
+        <v>0.63237849999999995</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2670,8 +2688,8 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <f>0.8*Phase1!B39</f>
-        <v>1.4000000000000001E-4</v>
+        <f>0.9*Phase1!B39</f>
+        <v>1.5750000000000001E-4</v>
       </c>
       <c r="D39">
         <f>1.05*Phase1!C39</f>
@@ -2679,7 +2697,7 @@
       </c>
       <c r="E39">
         <f t="shared" si="2"/>
-        <v>0.26485999999999998</v>
+        <v>0.26484249999999998</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2690,8 +2708,8 @@
         <v>1</v>
       </c>
       <c r="C40">
-        <f>0.8*Phase1!B40</f>
-        <v>1.6800000000000002E-4</v>
+        <f>0.9*Phase1!B40</f>
+        <v>1.8900000000000001E-4</v>
       </c>
       <c r="D40">
         <f>1.05*Phase1!C40</f>
@@ -2699,7 +2717,7 @@
       </c>
       <c r="E40">
         <f t="shared" si="2"/>
-        <v>0.26483200000000007</v>
+        <v>0.26481100000000002</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2710,8 +2728,8 @@
         <v>1</v>
       </c>
       <c r="C41">
-        <f>0.8*Phase1!B41</f>
-        <v>2.4399999999999999E-4</v>
+        <f>0.9*Phase1!B41</f>
+        <v>2.745E-4</v>
       </c>
       <c r="D41">
         <f>1.05*Phase1!C41</f>
@@ -2719,7 +2737,7 @@
       </c>
       <c r="E41">
         <f t="shared" si="2"/>
-        <v>0.26475599999999999</v>
+        <v>0.26472550000000006</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2730,12 +2748,12 @@
         <v>1</v>
       </c>
       <c r="C42">
-        <f>0.8*Phase1!B42</f>
-        <v>4.3200000000000004E-4</v>
+        <f>0.9*Phase1!B42</f>
+        <v>4.86E-4</v>
       </c>
       <c r="D42">
         <f>1-C42</f>
-        <v>0.99956800000000001</v>
+        <v>0.99951400000000001</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2751,8 +2769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2809,11 +2827,11 @@
         <v>-5.1099777374285189</v>
       </c>
       <c r="E2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F2">
         <f>LN(E2)</f>
-        <v>-0.2876820724517809</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="G2">
         <v>1.7000000000000001E-2</v>
@@ -2831,7 +2849,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="1">15*B3</f>
+        <f t="shared" ref="C3:C7" si="1">15*B3</f>
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D3">
@@ -2839,11 +2857,11 @@
         <v>-5.1099777374285189</v>
       </c>
       <c r="E3">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
         <f>LN(E3)</f>
-        <v>-0.2876820724517809</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="G3">
         <v>1.7000000000000001E-2</v>
@@ -2869,11 +2887,11 @@
         <v>-4.8853239920190807</v>
       </c>
       <c r="E4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F18" si="3">LN(E4)</f>
-        <v>-0.2876820724517809</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="G4">
         <v>3.0000000000000001E-3</v>
@@ -2899,11 +2917,11 @@
         <v>-4.7014899569937691</v>
       </c>
       <c r="E5">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="G5">
         <v>4.0000000000000001E-3</v>
@@ -2929,11 +2947,11 @@
         <v>-4.5458245078791428</v>
       </c>
       <c r="E6">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="G6">
         <v>3.0000000000000001E-3</v>
@@ -2959,11 +2977,11 @@
         <v>-4.4107760479598674</v>
       </c>
       <c r="E7">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G7">
         <v>3.0000000000000001E-3</v>
@@ -2981,19 +2999,19 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>1.35E-2</v>
+        <f>18*B8</f>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>-4.2914736400182862</v>
+        <v>-4.1064113821229009</v>
       </c>
       <c r="E8">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G8">
         <v>3.0000000000000001E-3</v>
@@ -3011,19 +3029,19 @@
         <v>1E-3</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <f>18*B9</f>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>-4.1845914400698785</v>
+        <v>-3.9992195504583012</v>
       </c>
       <c r="E9">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G9">
         <v>3.0000000000000001E-3</v>
@@ -3041,19 +3059,19 @@
         <v>1.8E-3</v>
       </c>
       <c r="C10">
-        <f>25*B10</f>
-        <v>4.4999999999999998E-2</v>
+        <f>26*B10</f>
+        <v>4.6800000000000001E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>-3.0550488507104103</v>
+        <v>-3.0139415423009859</v>
       </c>
       <c r="E10">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.51082562376599072</v>
       </c>
       <c r="G10">
         <v>3.0000000000000001E-3</v>
@@ -3071,19 +3089,19 @@
         <v>2E-3</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C18" si="4">25*B11</f>
-        <v>0.05</v>
+        <f t="shared" ref="C11:C18" si="4">26*B11</f>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>-2.9444389791664403</v>
+        <v>-2.9031107836735943</v>
       </c>
       <c r="E11">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.35667494393873245</v>
       </c>
       <c r="G11">
         <v>3.0000000000000001E-3</v>
@@ -3102,18 +3120,18 @@
       </c>
       <c r="C12">
         <f t="shared" si="4"/>
-        <v>0.1</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>-2.1972245773362191</v>
+        <v>-2.1535495138335579</v>
       </c>
       <c r="E12">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.35667494393873245</v>
       </c>
       <c r="G12">
         <v>3.0000000000000001E-3</v>
@@ -3132,18 +3150,18 @@
       </c>
       <c r="C13">
         <f t="shared" si="4"/>
-        <v>0.125</v>
+        <v>0.13</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>-1.9459101490553135</v>
+        <v>-1.900958761193047</v>
       </c>
       <c r="E13">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.35667494393873245</v>
       </c>
       <c r="G13">
         <v>1E-3</v>
@@ -3157,23 +3175,23 @@
       <c r="A14">
         <v>36</v>
       </c>
-      <c r="B14">
-        <v>7.0000000000000001E-3</v>
+      <c r="B14" s="6">
+        <v>0.01</v>
       </c>
       <c r="C14">
         <f t="shared" si="4"/>
-        <v>0.17500000000000002</v>
+        <v>0.26</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>-1.5505974124111668</v>
+        <v>-1.0459685551826876</v>
       </c>
       <c r="E14">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.35667494393873245</v>
       </c>
       <c r="G14">
         <v>1E-3</v>
@@ -3187,23 +3205,23 @@
       <c r="A15">
         <v>37</v>
       </c>
-      <c r="B15">
-        <v>8.0000000000000002E-3</v>
+      <c r="B15" s="6">
+        <v>0.01</v>
       </c>
       <c r="C15">
         <f t="shared" si="4"/>
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>-1.3862943611198906</v>
+        <v>-1.0459685551826876</v>
       </c>
       <c r="E15">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.22314355131420971</v>
       </c>
       <c r="G15">
         <v>1E-3</v>
@@ -3218,22 +3236,22 @@
         <v>38</v>
       </c>
       <c r="B16" s="6">
-        <v>8.9999999999999993E-3</v>
+        <v>0.01</v>
       </c>
       <c r="C16">
         <f t="shared" si="4"/>
-        <v>0.22499999999999998</v>
+        <v>0.26</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>-1.2367626271489269</v>
+        <v>-1.0459685551826876</v>
       </c>
       <c r="E16">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.22314355131420971</v>
       </c>
       <c r="G16">
         <v>1E-3</v>
@@ -3252,18 +3270,18 @@
       </c>
       <c r="C17">
         <f t="shared" si="4"/>
-        <v>0.27499999999999997</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>-0.9694005571881037</v>
+        <v>-0.91489115151973188</v>
       </c>
       <c r="E17">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.22314355131420971</v>
       </c>
       <c r="G17">
         <v>2E-3</v>
@@ -3282,18 +3300,18 @@
       </c>
       <c r="C18">
         <f t="shared" si="4"/>
-        <v>0.35000000000000003</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>-0.61903920840622328</v>
+        <v>-0.55804469570338155</v>
       </c>
       <c r="E18">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
-        <v>-0.2876820724517809</v>
+        <v>-0.22314355131420971</v>
       </c>
       <c r="G18">
         <v>1E-3</v>
@@ -3314,7 +3332,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3391,7 +3409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>

</xml_diff>